<commit_message>
Version quasi finale, problème de vies, de bouton et de filtre réglée !! Le bateau bouge comme un DIEU
</commit_message>
<xml_diff>
--- a/Codes/submarines/matrices.xlsx
+++ b/Codes/submarines/matrices.xlsx
@@ -3435,13 +3435,13 @@
   <dimension ref="A1:CH21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AW13" sqref="AW13"/>
+      <selection activeCell="AI26" sqref="AI26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.21875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="4.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="2" bestFit="1" customWidth="1"/>
     <col min="41" max="67" width="2.21875" style="5"/>
   </cols>
   <sheetData>
@@ -6273,6 +6273,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AU19:CH19"/>
+    <mergeCell ref="AU20:CH20"/>
+    <mergeCell ref="AU21:CH21"/>
+    <mergeCell ref="AU14:CH14"/>
+    <mergeCell ref="AU15:CH15"/>
+    <mergeCell ref="AU16:CH16"/>
+    <mergeCell ref="AU17:CH17"/>
+    <mergeCell ref="AU18:CH18"/>
     <mergeCell ref="A15:AN15"/>
     <mergeCell ref="A14:AN14"/>
     <mergeCell ref="A21:AN21"/>
@@ -6281,14 +6289,6 @@
     <mergeCell ref="A18:AN18"/>
     <mergeCell ref="A17:AN17"/>
     <mergeCell ref="A16:AN16"/>
-    <mergeCell ref="AU19:CH19"/>
-    <mergeCell ref="AU20:CH20"/>
-    <mergeCell ref="AU21:CH21"/>
-    <mergeCell ref="AU14:CH14"/>
-    <mergeCell ref="AU15:CH15"/>
-    <mergeCell ref="AU16:CH16"/>
-    <mergeCell ref="AU17:CH17"/>
-    <mergeCell ref="AU18:CH18"/>
   </mergeCells>
   <conditionalFormatting sqref="AQ1:AT7">
     <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">

</xml_diff>